<commit_message>
Added Motion Compensation data
</commit_message>
<xml_diff>
--- a/Experiments_Code/Static_Feature_Extraction_Experiment/Static_Experiment_Spreadsheet2.xlsx
+++ b/Experiments_Code/Static_Feature_Extraction_Experiment/Static_Experiment_Spreadsheet2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamin\Desktop\LiDAR_Motion_Comp_Feature_Extract_Repo\LiDAR-Motion-Compensation-and-Feature-Extraction\Experiments_Code\Static_Feature_Extraction_Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B272E807-8D57-4172-A55C-0286F384EF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EDCC9D-0BB9-4C73-8462-302C0C5C84D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8DE0EAC1-9958-4E98-B9E2-C08446E73EFF}"/>
   </bookViews>
@@ -156,7 +156,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5756,8 +5756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D77D76BA-A3D3-4E0F-AC14-4BB4AF25659D}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38:K48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>